<commit_message>
add explain plans and fix query 21
</commit_message>
<xml_diff>
--- a/sgd_assignment1_tables&graphs.xlsx
+++ b/sgd_assignment1_tables&graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\OneDrive\Ambiente de Trabalho\SGD-TPCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87673813-0BF9-467E-9EC0-09150F0C020C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7AB115-B970-44B1-AEED-E4AEF91E1281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{247B33D0-6AB8-40A3-8C41-44B27BA98C90}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="85">
   <si>
     <t>Q1</t>
   </si>
@@ -295,9 +295,6 @@
   <si>
     <t>Rows</t>
   </si>
-  <si>
-    <t>Absolutely, here's the data formatted as a Google Sheets table, similar to the previous one:</t>
-  </si>
 </sst>
 </file>
 
@@ -494,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,11 +546,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4239,7 +4246,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2579.5950824419601</c:v>
+                  <c:v>254.94487826328483</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>52.929609457651736</c:v>
@@ -4358,70 +4365,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>189.25566384792305</c:v>
+                  <c:v>354.75388593673637</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.825162124633742</c:v>
+                  <c:v>13.082218980789099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>546.38418822288179</c:v>
+                  <c:v>1264.7146480560259</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.21389079093898</c:v>
+                  <c:v>136.92517867088281</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>322.23930556774127</c:v>
+                  <c:v>756.47693457603395</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.986880850791906</c:v>
+                  <c:v>129.49137730598397</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>243.76486344337442</c:v>
+                  <c:v>513.80241379737822</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138.58812627792338</c:v>
+                  <c:v>391.28609972000061</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1174.6765144586552</c:v>
+                  <c:v>2373.3484481811456</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110.68573498725866</c:v>
+                  <c:v>340.07605986595098</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35.987437081336964</c:v>
+                  <c:v>160.04542603492678</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>81.273595142364229</c:v>
+                  <c:v>153.68513107299742</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>799.30343711375951</c:v>
+                  <c:v>1831.436336565014</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>71.573976969718728</c:v>
+                  <c:v>137.20876836776702</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.890755534172033</c:v>
+                  <c:v>1.138963699340814E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>56.817186594009129</c:v>
+                  <c:v>132.3307879447934</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>48.211100912094047</c:v>
+                  <c:v>67.029065704345655</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>168.58993432521774</c:v>
+                  <c:v>129.50369310378977</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40.000493073463403</c:v>
+                  <c:v>70.392898368835375</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>176.41999056339242</c:v>
+                  <c:v>294.2160739898676</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1541.4275218486766</c:v>
+                  <c:v>419.80496568679763</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.567874860763521</c:v>
+                  <c:v>14.60571494102474</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4875,7 +4882,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2641.4571911334961</c:v>
+                  <c:v>170.32293924419997</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>10.802513551712023</c:v>
@@ -10798,8 +10805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5F3338-F5F4-46D3-A61E-670C9DC8D3B7}">
   <dimension ref="B8:Q96"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10818,17 +10825,17 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -11729,17 +11736,17 @@
       <c r="N37" s="6"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
@@ -12992,8 +12999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739F7174-EA87-44DE-A404-B76B78C6C87E}">
   <dimension ref="C5:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37:J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13010,17 +13017,17 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
@@ -13800,17 +13807,17 @@
       <c r="K34" s="6"/>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="7" t="s">
@@ -14535,10 +14542,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F367539-F476-4269-9596-D1A2C0F3D96F}">
-  <dimension ref="C5:Q58"/>
+  <dimension ref="C5:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14555,725 +14562,726 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="22" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="19">
         <v>64.0001540184021</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="19">
         <v>57.860941886901799</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="19">
         <v>66.376424551010103</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="19">
         <v>66.112741708755493</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="19">
         <v>62.3278038501739</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="19">
         <v>69.581334352493201</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="23">
         <f>AVERAGE(D7:H7)</f>
         <v>63.33561320304868</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="23">
         <f>_xlfn.STDEV.P(D7:H7)</f>
         <v>3.1108936528899287</v>
       </c>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="19">
         <v>11.2891526222229</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="19">
         <v>10.1152460575103</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="19">
         <v>11.800162315368601</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="19">
         <v>11.8232951164245</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="19">
         <v>15.1887099742889</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="19">
         <v>12.4443078041076</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="23">
         <f t="shared" ref="J8:J28" si="0">AVERAGE(D8:H8)</f>
         <v>12.043313217163041</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="23">
         <f t="shared" ref="K8:K28" si="1">_xlfn.STDEV.P(D8:H8)</f>
         <v>1.6903994948251526</v>
       </c>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="19">
         <v>30.116919994354198</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="19">
         <v>28.070521354675201</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="19">
         <v>31.2290291786193</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="19">
         <v>30.851280927657999</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="19">
         <v>31.0562324523925</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="19">
         <v>30.2217309474945</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="23">
         <f t="shared" si="0"/>
         <v>30.264796781539836</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="23">
         <f t="shared" si="1"/>
         <v>1.1607575443178382</v>
       </c>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="19">
         <v>39.680542945861802</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="19">
         <v>35.463392257690401</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="19">
         <v>36.985944271087597</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="19">
         <v>41.9373681545257</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="19">
         <v>56.703636884689303</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="19">
         <v>37.811415672302203</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="23">
         <f t="shared" si="0"/>
         <v>42.154176902770963</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="23">
         <f t="shared" si="1"/>
         <v>7.6069689686967275</v>
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="19">
         <v>30.457514047622599</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="19">
         <v>28.155177831649699</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="19">
         <v>29.715933084487901</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="19">
         <v>36.1554563045501</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="19">
         <v>32.279606580734203</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="19">
         <v>29.5882954597473</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="23">
         <f t="shared" si="0"/>
         <v>31.352737569808902</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="23">
         <f t="shared" si="1"/>
         <v>2.7433605583439848</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="19">
         <v>22.3648827075958</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="19">
         <v>20.411009311676001</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="19">
         <v>20.4435920715332</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="19">
         <v>25.230216264724699</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="19">
         <v>24.142680406570399</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="19">
         <v>20.739531755447299</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="23">
         <f t="shared" si="0"/>
         <v>22.518476152420021</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="23">
         <f t="shared" si="1"/>
         <v>1.9370970691283635</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="19">
         <v>29.969155311584402</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="19">
         <v>27.050234556198099</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="19">
         <v>27.560783147811801</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="19">
         <v>34.336606740951503</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="19">
         <v>30.993014812469401</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="19">
         <v>28.384186267852701</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="23">
         <f t="shared" si="0"/>
         <v>29.981958913803037</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="23">
         <f t="shared" si="1"/>
         <v>2.6245935098503925</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="19">
         <v>30.421542882919301</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="19">
         <v>27.330114364623999</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="19">
         <v>27.944201707839898</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="19">
         <v>34.355662822723303</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="19">
         <v>32.666440963745103</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="19">
         <v>28.029461622238099</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="23">
         <f t="shared" si="0"/>
         <v>30.54359254837032</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="23">
         <f t="shared" si="1"/>
         <v>2.6883651564230844</v>
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="19">
         <v>45.235015153884802</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="19">
         <v>39.440730810165398</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="19">
         <v>43.998061180114703</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="19">
         <v>56.277429580688398</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="19">
         <v>62.6246078014373</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="19">
         <v>47.013283252716001</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="23">
         <f t="shared" si="0"/>
         <v>49.515168905258122</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="23">
         <f t="shared" si="1"/>
         <v>8.5771563391745858</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="19">
         <v>31.439683914184499</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="19">
         <v>28.5523147583007</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="19">
         <v>31.512265920638999</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="19">
         <v>36.5184390544891</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="19">
         <v>33.110831737518303</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="19">
         <v>31.127403974532999</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="23">
         <f t="shared" si="0"/>
         <v>32.226707077026319</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="23">
         <f t="shared" si="1"/>
         <v>2.6012162662249398</v>
       </c>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C17" s="7" t="s">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="19">
         <v>6.5764472484588596</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="19">
         <v>6.01344871520996</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="19">
         <v>6.65913534164428</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="19">
         <v>8.2712528705596906</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="19">
         <v>8.1299188137054408</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="19">
         <v>6.6061971187591499</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="23">
         <f t="shared" si="0"/>
         <v>7.1300405979156469</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="23">
         <f t="shared" si="1"/>
         <v>0.90300793873756813</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C18" s="7" t="s">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="19">
         <v>28.579901933670001</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="19">
         <v>25.055998563766401</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="19">
         <v>28.8946788311004</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="19">
         <v>33.533298254012998</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="19">
         <v>32.538560390472398</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="19">
         <v>27.9399654865264</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="23">
         <f t="shared" si="0"/>
         <v>29.720487594604435</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="23">
         <f t="shared" si="1"/>
         <v>3.0403754074103744</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C19" s="7" t="s">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="19">
         <v>58.004550218582096</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="19">
         <v>50.908254146575899</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="19">
         <v>60.4556596279144</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="19">
         <v>72.7278985977172</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="19">
         <v>68.860414505004798</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="19">
         <v>62.515816450118997</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="23">
         <f t="shared" si="0"/>
         <v>62.191355419158882</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="23">
         <f t="shared" si="1"/>
         <v>7.7890364389802391</v>
       </c>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C20" s="7" t="s">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="19">
         <v>19.637489080428999</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="19">
         <v>18.720854520797701</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="19">
         <v>18.739871025085399</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="19">
         <v>21.149337530136101</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="19">
         <v>23.4136755466461</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="19">
         <v>19.120045185089101</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="23">
         <f t="shared" si="0"/>
         <v>20.33224554061886</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="23">
         <f t="shared" si="1"/>
         <v>1.7763881533513179</v>
       </c>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C21" s="7" t="s">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="19">
         <v>37.056133508682201</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="19">
         <v>35.274138450622502</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="19">
         <v>36.964099168777402</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="19">
         <v>38.189855575561502</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="19">
         <v>41.336944103240903</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="19">
         <v>35.996903181076</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="23">
         <f t="shared" si="0"/>
         <v>37.764234161376905</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="23">
         <f t="shared" si="1"/>
         <v>2.0143291243663581</v>
       </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="19">
         <v>10.0704312324523</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="19">
         <v>8.5204789638519198</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="19">
         <v>9.8714163303375209</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="19">
         <v>10.5706801414489</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="19">
         <v>12.559695005416801</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="19">
         <v>10.032133579254101</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="23">
         <f t="shared" si="0"/>
         <v>10.318540334701488</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="23">
         <f t="shared" si="1"/>
         <v>1.310026826859237</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C23" s="7" t="s">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7">
+      <c r="D23" s="19">
         <v>0</v>
       </c>
-      <c r="F23" s="7">
+      <c r="E23" s="19">
         <v>0</v>
       </c>
-      <c r="G23" s="7">
+      <c r="F23" s="19">
         <v>0</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7">
+      <c r="G23" s="19">
         <v>0</v>
       </c>
-      <c r="J23" s="9">
+      <c r="H23" s="19"/>
+      <c r="I23" s="19">
+        <v>0</v>
+      </c>
+      <c r="J23" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C24" s="7" t="s">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="19">
         <v>221.913088321685</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="19">
         <v>216.57733273506099</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="19">
         <v>242.10486268997099</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="19">
         <v>230.458415985107</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="19">
         <v>284.67760705947802</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="19">
         <v>221.21555423736501</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="23">
         <f t="shared" si="0"/>
         <v>239.14626135826038</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="23">
         <f t="shared" si="1"/>
         <v>24.346146358466026</v>
       </c>
-      <c r="Q24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="19">
         <v>19.472764492034901</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="19">
         <v>20.865331172943101</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="19">
         <v>21.047028541564899</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="19">
         <v>22.2864732742309</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="19">
         <v>22.356169462203901</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="19">
         <v>21.300621032714801</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="23">
         <f t="shared" si="0"/>
         <v>21.20555338859554</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="23">
         <f t="shared" si="1"/>
         <v>1.0616726229117204</v>
       </c>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C26" s="7" t="s">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7">
+      <c r="D26" s="19">
         <v>0</v>
       </c>
-      <c r="F26" s="7">
+      <c r="E26" s="19">
         <v>0</v>
       </c>
-      <c r="G26" s="7">
+      <c r="F26" s="19">
         <v>0</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7">
+      <c r="G26" s="19">
         <v>0</v>
       </c>
-      <c r="J26" s="9">
+      <c r="H26" s="19"/>
+      <c r="I26" s="19">
+        <v>0</v>
+      </c>
+      <c r="J26" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C27" s="7" t="s">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="7">
-        <v>2446.8583312034598</v>
-      </c>
-      <c r="E27" s="7">
-        <v>2484.6778788566498</v>
-      </c>
-      <c r="F27" s="7">
-        <v>2907.15026760101</v>
-      </c>
-      <c r="G27" s="7">
-        <v>2768.7846627235399</v>
-      </c>
-      <c r="H27" s="7">
-        <v>2599.8148152828198</v>
-      </c>
-      <c r="I27" s="7">
-        <v>2913.2283632755202</v>
-      </c>
-      <c r="J27" s="9">
+      <c r="D27" s="19">
+        <v>170.32480161800001</v>
+      </c>
+      <c r="E27" s="19">
+        <v>168.67221450700001</v>
+      </c>
+      <c r="F27" s="19">
+        <v>173.89773677299999</v>
+      </c>
+      <c r="G27" s="19">
+        <v>168.26965442700001</v>
+      </c>
+      <c r="H27" s="19">
+        <v>170.45028889599999</v>
+      </c>
+      <c r="I27" s="19">
+        <v>174.669687186</v>
+      </c>
+      <c r="J27" s="23">
         <f t="shared" si="0"/>
-        <v>2641.4571911334961</v>
-      </c>
-      <c r="K27" s="9">
+        <v>170.32293924419997</v>
+      </c>
+      <c r="K27" s="23">
         <f t="shared" si="1"/>
-        <v>173.77436658773661</v>
-      </c>
-    </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C28" s="7" t="s">
+        <v>1.9867697135154982</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="19">
         <v>9.3544542789459193</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="19">
         <v>11.0285313129425</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="19">
         <v>11.247937202453601</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="19">
         <v>11.8857760429382</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="19">
         <v>10.4958689212799</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="19">
         <v>12.607521772384599</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="23">
         <f t="shared" si="0"/>
         <v>10.802513551712023</v>
       </c>
-      <c r="K28" s="9">
+      <c r="K28" s="23">
         <f t="shared" si="1"/>
         <v>0.85015886383027095</v>
       </c>
     </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -15284,7 +15292,7 @@
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -15295,7 +15303,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -15306,7 +15314,7 @@
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -15340,17 +15348,17 @@
       <c r="K34" s="6"/>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="7" t="s">
@@ -16005,31 +16013,31 @@
       <c r="C57" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="19">
-        <v>2599.6444351673099</v>
+      <c r="D57">
+        <v>254.96321797370899</v>
       </c>
       <c r="E57" s="19">
-        <v>2599.7643129825501</v>
+        <v>250.963217974</v>
       </c>
       <c r="F57" s="19">
-        <v>2566.8376481533001</v>
+        <v>254.963217974</v>
       </c>
       <c r="G57" s="19">
-        <v>2584.75719571113</v>
+        <v>250.85317971200001</v>
       </c>
       <c r="H57" s="19">
-        <v>2536.6981668472199</v>
+        <v>258.963217972</v>
       </c>
       <c r="I57" s="19">
-        <v>2589.86873579025</v>
+        <v>258.96321797399997</v>
       </c>
       <c r="J57" s="9">
         <f t="shared" si="2"/>
-        <v>2579.5950824419601</v>
+        <v>254.94487826328483</v>
       </c>
       <c r="K57" s="9">
         <f t="shared" si="3"/>
-        <v>22.150497620449638</v>
+        <v>3.2886267759549956</v>
       </c>
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.25">
@@ -16077,8 +16085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB0DE57-CC1C-42F4-9D16-9132C59C104F}">
   <dimension ref="B2:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16091,13 +16099,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
@@ -16269,11 +16277,11 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
@@ -16385,11 +16393,11 @@
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="24"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
@@ -16504,35 +16512,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84608353-83C5-4835-B580-A120DB25BDA7}">
   <dimension ref="B3:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
     <col min="14" max="14" width="20.5703125" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
@@ -16573,8 +16582,7 @@
         <v>109.16129084428115</v>
       </c>
       <c r="H5" s="9">
-        <f>AVERAGE(B5:F5)</f>
-        <v>189.25566384792305</v>
+        <v>354.75388593673637</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -16595,8 +16603,7 @@
         <v>22.587079962094588</v>
       </c>
       <c r="H6" s="9">
-        <f t="shared" ref="H6:H26" si="0">AVERAGE(B6:F6)</f>
-        <v>10.825162124633742</v>
+        <v>13.082218980789099</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -16617,8 +16624,7 @@
         <v>65.364525357882101</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" si="0"/>
-        <v>546.38418822288179</v>
+        <v>1264.7146480560259</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -16639,8 +16645,7 @@
         <v>68.793136835098224</v>
       </c>
       <c r="H8" s="9">
-        <f t="shared" si="0"/>
-        <v>100.21389079093898</v>
+        <v>136.92517867088281</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -16661,8 +16666,7 @@
         <v>65.004720250765388</v>
       </c>
       <c r="H9" s="9">
-        <f t="shared" si="0"/>
-        <v>322.23930556774127</v>
+        <v>756.47693457603395</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -16683,8 +16687,7 @@
         <v>66.386156717936132</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" si="0"/>
-        <v>56.986880850791906</v>
+        <v>129.49137730598397</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -16705,8 +16708,7 @@
         <v>52.922709345817537</v>
       </c>
       <c r="H11" s="9">
-        <f t="shared" si="0"/>
-        <v>243.76486344337442</v>
+        <v>513.80241379737822</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -16727,8 +16729,7 @@
         <v>55.853649298349985</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" si="0"/>
-        <v>138.58812627792338</v>
+        <v>391.28609972000061</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -16749,8 +16750,7 @@
         <v>99.51390922069497</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" si="0"/>
-        <v>1174.6765144586552</v>
+        <v>2373.3484481811456</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -16771,8 +16771,7 @@
         <v>65.464872876802986</v>
       </c>
       <c r="H14" s="9">
-        <f t="shared" si="0"/>
-        <v>110.68573498725866</v>
+        <v>340.07605986595098</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -16793,8 +16792,7 @@
         <v>15.19534341494238</v>
       </c>
       <c r="H15" s="9">
-        <f t="shared" si="0"/>
-        <v>35.987437081336964</v>
+        <v>160.04542603492678</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -16815,8 +16813,7 @@
         <v>62.032307187716121</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" si="0"/>
-        <v>81.273595142364229</v>
+        <v>153.68513107299742</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -16837,8 +16834,7 @@
         <v>81.264069875081219</v>
       </c>
       <c r="H17" s="9">
-        <f t="shared" si="0"/>
-        <v>799.30343711375951</v>
+        <v>1831.436336565014</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -16859,8 +16855,7 @@
         <v>34.734125415484051</v>
       </c>
       <c r="H18" s="9">
-        <f t="shared" si="0"/>
-        <v>71.573976969718728</v>
+        <v>137.20876836776702</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -16881,8 +16876,7 @@
         <v>98.61200451850884</v>
       </c>
       <c r="H19" s="9">
-        <f t="shared" si="0"/>
-        <v>18.890755534172033</v>
+        <v>1.138963699340814E-2</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -16903,8 +16897,7 @@
         <v>18.053256114323869</v>
       </c>
       <c r="H20" s="9">
-        <f t="shared" si="0"/>
-        <v>56.817186594009129</v>
+        <v>132.3307879447934</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -16925,8 +16918,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="9">
-        <f t="shared" si="0"/>
-        <v>48.211100912094047</v>
+        <v>67.029065704345655</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -16947,8 +16939,7 @@
         <v>279.53225533167466</v>
       </c>
       <c r="H22" s="9">
-        <f t="shared" si="0"/>
-        <v>168.58993432521774</v>
+        <v>129.50369310378977</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -16969,8 +16960,7 @@
         <v>46.160212278366053</v>
       </c>
       <c r="H23" s="9">
-        <f t="shared" si="0"/>
-        <v>40.000493073463403</v>
+        <v>70.392898368835375</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -16991,8 +16981,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="9">
-        <f t="shared" si="0"/>
-        <v>176.41999056339242</v>
+        <v>294.2160739898676</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -17000,7 +16989,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="9">
-        <v>2641.4571911334961</v>
+        <v>170.32293924419997</v>
       </c>
       <c r="D25" s="9">
         <v>441.39785256385738</v>
@@ -17010,11 +16999,10 @@
         <v>20</v>
       </c>
       <c r="G25" s="9">
-        <v>2579.5950824419601</v>
+        <v>254.94487826328483</v>
       </c>
       <c r="H25" s="9">
-        <f t="shared" si="0"/>
-        <v>1541.4275218486766</v>
+        <v>419.80496568679763</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -17035,8 +17023,7 @@
         <v>52.929609457651736</v>
       </c>
       <c r="H26" s="9">
-        <f t="shared" si="0"/>
-        <v>11.567874860763521</v>
+        <v>14.60571494102474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>